<commit_message>
JSON read ok but needs improvement
</commit_message>
<xml_diff>
--- a/ATK_P1 Task View.xlsx
+++ b/ATK_P1 Task View.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\005_Java\adam-kager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8C3C37-701D-48A9-BF24-DCD7DFC6450E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1954CF-C7B9-45CD-BFDE-8AE38B7CD1AE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1872" yWindow="324" windowWidth="15288" windowHeight="11748" xr2:uid="{A4DBBC63-E219-43C4-A775-3E37E3D0067B}"/>
+    <workbookView xWindow="-192" yWindow="276" windowWidth="15288" windowHeight="11748" xr2:uid="{A4DBBC63-E219-43C4-A775-3E37E3D0067B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="66">
   <si>
     <t>User-Stories</t>
   </si>
@@ -227,13 +227,16 @@
   </si>
   <si>
     <t>Updata</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,6 +268,20 @@
       <name val="Lucida Console"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -286,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -308,6 +325,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -625,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47BD7B20-6072-4F89-8E94-4D6028DB5A62}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -656,7 +679,9 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="C3" s="4">
         <v>1</v>
       </c>
@@ -667,7 +692,9 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="C4" s="4">
         <f>C3+1</f>
         <v>2</v>
@@ -679,7 +706,9 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="C5" s="4">
         <f t="shared" ref="C5:C23" si="0">C4+1</f>
         <v>3</v>
@@ -739,13 +768,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="6" t="s">
+      <c r="D10" s="8"/>
+      <c r="E10" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -763,7 +792,9 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
+      <c r="B12" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="C12" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -787,7 +818,9 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="C14" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -903,7 +936,9 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
+      <c r="B24" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="C24" s="4">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
adding to employee info page
</commit_message>
<xml_diff>
--- a/ATK_P1 Task View.xlsx
+++ b/ATK_P1 Task View.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\005_Java\adam-kager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1954CF-C7B9-45CD-BFDE-8AE38B7CD1AE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CACA75F-3E3A-4521-BFBE-13C1E1226093}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-192" yWindow="276" windowWidth="15288" windowHeight="11748" xr2:uid="{A4DBBC63-E219-43C4-A775-3E37E3D0067B}"/>
+    <workbookView xWindow="348" yWindow="588" windowWidth="15288" windowHeight="11748" xr2:uid="{A4DBBC63-E219-43C4-A775-3E37E3D0067B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
   <si>
     <t>User-Stories</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>x*</t>
   </si>
 </sst>
 </file>
@@ -303,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -331,6 +334,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -649,7 +655,7 @@
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A13" sqref="A13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -768,7 +774,9 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="8"/>
+      <c r="B10" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="C10" s="8">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -805,14 +813,14 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="7" t="s">
+      <c r="D13" s="8"/>
+      <c r="E13" s="10" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added view all employees to manager profile page
</commit_message>
<xml_diff>
--- a/ATK_P1 Task View.xlsx
+++ b/ATK_P1 Task View.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\005_Java\adam-kager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59A4533-CB81-49CD-8843-C02E1B3C3961}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9552E83C-15DA-4BDB-881D-53ACA9D839BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="348" yWindow="588" windowWidth="15288" windowHeight="11748" xr2:uid="{A4DBBC63-E219-43C4-A775-3E37E3D0067B}"/>
+    <workbookView xWindow="444" yWindow="504" windowWidth="15288" windowHeight="11748" xr2:uid="{A4DBBC63-E219-43C4-A775-3E37E3D0067B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="66">
   <si>
     <t>User-Stories</t>
   </si>
@@ -648,7 +648,7 @@
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -873,9 +873,11 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>0</v>
-      </c>
-      <c r="B16" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="C16" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -901,9 +903,11 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>0</v>
-      </c>
-      <c r="B18" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="C18" s="4">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -915,9 +919,11 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>0</v>
-      </c>
-      <c r="B19" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="C19" s="4">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -979,7 +985,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>65</v>
@@ -995,11 +1001,11 @@
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <f>SUM(A3:A24)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C25" s="8">
         <f>A25/C24</f>
-        <v>0.33333333333333331</v>
+        <v>0.52380952380952384</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1379,7 +1385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88441CD3-C8CB-43EF-8C75-4BA13CEF4CB7}">
   <dimension ref="C3:C55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="C8" sqref="C8:D16"/>
     </sheetView>
   </sheetViews>

</xml_diff>